<commit_message>
solved search in rotated osrted array, 3 sum num and container with most water
</commit_message>
<xml_diff>
--- a/Leetcode 75 Questions.xlsx
+++ b/Leetcode 75 Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding_interview_prep\coding_interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827D270C-11BC-421E-BBFE-B191652CDA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CB63F4-2636-4FAD-8DBB-2B5370B95233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="326">
   <si>
     <t>Video Solution</t>
   </si>
@@ -991,6 +991,15 @@
   </si>
   <si>
     <t xml:space="preserve">modified binary search, to break condition check if mid &gt; mid +1 then return mid + 1, check if mid &lt; mid -1 then return mid, to increase left or decrease right compare mid with array at 0 if mid &gt; arr[0] then left = mid +1  if mid &lt; arry[0] right = right -1 </t>
+  </si>
+  <si>
+    <t>find min value with modified binary search, and then do two binary search, from 0 to min_idx -1 and from min_idx until len(arr)</t>
+  </si>
+  <si>
+    <t>sort the array in place, start at the beginnning and check if curr_num is equl to previous num if it is continue to avoid duplicates, then initialzie left and right pointer, check num + left + right = target and append this values to list, then increment left_pointer until num[left] != num[left - 1]</t>
+  </si>
+  <si>
+    <t>left = 0, right = len(arr) - 1, start computing the area=min(height[l], height[r]) * (r - l), max_area = max(max_area, area), if left &lt;= right left += 1 else right -= 1</t>
   </si>
 </sst>
 </file>
@@ -1516,8 +1525,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1678,7 +1687,9 @@
       <c r="D9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -1693,7 +1704,9 @@
       <c r="D10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1708,7 +1721,9 @@
       <c r="D11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -5635,8 +5650,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
solved problems with bith manipulation and started dynamic programing
</commit_message>
<xml_diff>
--- a/Leetcode 75 Questions.xlsx
+++ b/Leetcode 75 Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding_interview_prep\coding_interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CB63F4-2636-4FAD-8DBB-2B5370B95233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66D50D1-CF77-480C-8B83-027A29EEABC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="330">
   <si>
     <t>Video Solution</t>
   </si>
@@ -1000,13 +1000,26 @@
   </si>
   <si>
     <t>left = 0, right = len(arr) - 1, start computing the area=min(height[l], height[r]) * (r - l), max_area = max(max_area, area), if left &lt;= right left += 1 else right -= 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create mask=0xffffffff , while (b &amp; mask): carry =(a &amp; b) &lt;&lt; 1,  a= a ^ b, b = carry return a &amp; mask if b &gt; 0 else a, this handles overflow and negative numbers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">you can mod the number with 2 to get remainder and see if this is a 1 bit, then shift the num to the right once, while n &gt; 0 : count += n % 2 n = n &gt;&gt; 1 </t>
+  </si>
+  <si>
+    <t>Do an and with 1 and then move this bit left one position and do an or with the next result</t>
+  </si>
+  <si>
+    <t>use dynamic programing, base case is 0 and you see that you are repeating everytime the same computation, so you use offset to go back from the most significant bit, for this you check if off_set*2== i then you off_set*=2 and the ans[i] = 1 + ans[i - off_set]
+write out result for num=16 to figure out pattern; res[i] = res[i - offset], where offset is the biggest power of 2 &lt;= I;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1122,6 +1135,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1271,10 +1290,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1305,8 +1325,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1525,8 +1550,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1738,9 +1763,11 @@
       <c r="D12" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="4"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E12" s="4" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>40</v>
       </c>
@@ -1753,9 +1780,11 @@
       <c r="D13" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="4"/>
-    </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E13" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>43</v>
       </c>
@@ -1765,10 +1794,12 @@
       <c r="C14" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="4"/>
+      <c r="E14" s="23" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -1783,7 +1814,9 @@
       <c r="D15" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="4" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1798,7 +1831,9 @@
       <c r="D16" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -1813,7 +1848,9 @@
       <c r="D17" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -5651,7 +5688,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
worked on dynamic programing problems
</commit_message>
<xml_diff>
--- a/Leetcode 75 Questions.xlsx
+++ b/Leetcode 75 Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding_interview_prep\coding_interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66D50D1-CF77-480C-8B83-027A29EEABC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709DA23C-EA1F-4B62-B991-52A82FD700B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="334">
   <si>
     <t>Video Solution</t>
   </si>
@@ -1013,6 +1013,18 @@
   <si>
     <t>use dynamic programing, base case is 0 and you see that you are repeating everytime the same computation, so you use offset to go back from the most significant bit, for this you check if off_set*2== i then you off_set*=2 and the ans[i] = 1 + ans[i - off_set]
 write out result for num=16 to figure out pattern; res[i] = res[i - offset], where offset is the biggest power of 2 &lt;= I;</t>
+  </si>
+  <si>
+    <t>top-down:recursive solution, store amount in cache and for each coin call same function(amount - coin) and at the end add + 1 if solution is different than inf; bottom-up: compute coins for amount = 1, up until n, using for each coin (amount - coin), cache prev values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start at the end with 1, then go back by one and check if next numbers are bigger than current num, if so read previous value and increase by 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">create a matrix of str1 and str2 with empty array to have this as base case, and then check if the value in row is equal to value in right then increase value by one, if they are not the same take the max of the previous col or the previous row </t>
+  </si>
+  <si>
+    <t>recursive approach, start at index i and compare for each wor di the word is in the string[i: I + len(word)] if it is call again the function and check if return is tru to save in cache, return True if i &gt;= len(s) otherwise return false, for dynamic you need to have a dp array of len(s) + 1 and base case is true, then you compare s[i - len(word):i] == word: dp[i] = dp[i - len(word)] and return dp[-1]</t>
   </si>
 </sst>
 </file>
@@ -1550,8 +1562,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1865,7 +1877,9 @@
       <c r="D18" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
@@ -1877,10 +1891,12 @@
       <c r="C19" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="4"/>
+      <c r="E19" s="4" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -1895,7 +1911,9 @@
       <c r="D20" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="4"/>
+      <c r="E20" s="4" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -1910,7 +1928,9 @@
       <c r="D21" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
@@ -5687,8 +5707,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
longest increasing subsequence and working on dynamic programing problems
</commit_message>
<xml_diff>
--- a/Leetcode 75 Questions.xlsx
+++ b/Leetcode 75 Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding_interview_prep\coding_interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{709DA23C-EA1F-4B62-B991-52A82FD700B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3C3BB6-52AD-448C-9605-059A317F7449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="335">
   <si>
     <t>Video Solution</t>
   </si>
@@ -1025,6 +1025,9 @@
   </si>
   <si>
     <t>recursive approach, start at index i and compare for each wor di the word is in the string[i: I + len(word)] if it is call again the function and check if return is tru to save in cache, return True if i &gt;= len(s) otherwise return false, for dynamic you need to have a dp array of len(s) + 1 and base case is true, then you compare s[i - len(word):i] == word: dp[i] = dp[i - len(word)] and return dp[-1]</t>
+  </si>
+  <si>
+    <t>recursive approach, draw tree from start minus candidates, when 0 append to the final list, if candiates is bigger than target break loop</t>
   </si>
 </sst>
 </file>
@@ -1563,7 +1566,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1945,7 +1948,9 @@
       <c r="D22" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="4" t="s">
+        <v>334</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">

</xml_diff>

<commit_message>
finish with the dynamic programing questions
</commit_message>
<xml_diff>
--- a/Leetcode 75 Questions.xlsx
+++ b/Leetcode 75 Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding_interview_prep\coding_interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3C3BB6-52AD-448C-9605-059A317F7449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E595C6C-942D-4D39-8FC3-1B5E58AE6FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="340">
   <si>
     <t>Video Solution</t>
   </si>
@@ -1028,6 +1028,21 @@
   </si>
   <si>
     <t>recursive approach, draw tree from start minus candidates, when 0 append to the final list, if candiates is bigger than target break loop</t>
+  </si>
+  <si>
+    <t>first approach is no initialize dp array and then get the max(dp[i-2] + num[i], dp[i-1]) meaning max value so far excluding previous house or including previous house</t>
+  </si>
+  <si>
+    <t>same approach of house robber 1 but excluding first house and then excluding last house</t>
+  </si>
+  <si>
+    <t xml:space="preserve">can cur char be decoded in one or two ways? Recursion -&gt; cache -&gt; iterative dp solution, if char is 0 return 0, move by 1 and if possible to move by 2(next two chars ar valid 1-26) also move by two </t>
+  </si>
+  <si>
+    <t xml:space="preserve">create grid and sum previous col and previous row for dp approach </t>
+  </si>
+  <si>
+    <t xml:space="preserve">initialize right pointer at the end of array and iterate backwards in the nums cheking if you can reach right pointer, if true update right pointer to current pos and return true if last pointer is 0 </t>
   </si>
 </sst>
 </file>
@@ -1565,8 +1580,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1965,7 +1980,9 @@
       <c r="D23" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E23" s="4"/>
+      <c r="E23" s="4" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
@@ -1980,7 +1997,9 @@
       <c r="D24" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="E24" s="4"/>
+      <c r="E24" s="4" t="s">
+        <v>336</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
@@ -1995,7 +2014,9 @@
       <c r="D25" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E25" s="4"/>
+      <c r="E25" s="4" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -2010,7 +2031,9 @@
       <c r="D26" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="E26" s="4"/>
+      <c r="E26" s="4" t="s">
+        <v>338</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
@@ -2025,7 +2048,9 @@
       <c r="D27" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="E27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -5712,8 +5737,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
working on graph problems
</commit_message>
<xml_diff>
--- a/Leetcode 75 Questions.xlsx
+++ b/Leetcode 75 Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding_interview_prep\coding_interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E595C6C-942D-4D39-8FC3-1B5E58AE6FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA61E5E-F024-49A0-B39E-BCDF1CEFF7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="343">
   <si>
     <t>Video Solution</t>
   </si>
@@ -1043,6 +1043,16 @@
   </si>
   <si>
     <t xml:space="preserve">initialize right pointer at the end of array and iterate backwards in the nums cheking if you can reach right pointer, if true update right pointer to current pos and return true if last pointer is 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">recursive dfs, hashmap for visited nodes and append neigh for each node visited </t>
+  </si>
+  <si>
+    <t xml:space="preserve">create a course map to have prerequisistes, create a visit set to check for loops, do a dfs at each course and check if you can finish the prereq of each course recursive, if one is False return False directl </t>
+  </si>
+  <si>
+    <t>start from rows and cols that are directly connected to the oceans, set_atl, set_pac and do a dfs from this positions, then return a position if is in both set_a and set_p 
+dfs each cell, keep track of visited, and track which reach pac, atl; dfs on cells adjacent to pac, atl, find overlap of cells that are visited by both pac and atl cells;</t>
   </si>
 </sst>
 </file>
@@ -1580,8 +1590,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="D15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2065,7 +2075,9 @@
       <c r="D28" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="E28" s="4"/>
+      <c r="E28" s="4" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
@@ -2080,9 +2092,11 @@
       <c r="D29" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="E29" s="4"/>
-    </row>
-    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E29" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>93</v>
       </c>
@@ -2095,7 +2109,9 @@
       <c r="D30" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E30" s="4"/>
+      <c r="E30" s="23" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
@@ -5738,7 +5754,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
working on problems at needcode.io and updating comments on solutions
</commit_message>
<xml_diff>
--- a/Leetcode 75 Questions.xlsx
+++ b/Leetcode 75 Questions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding_interview_prep\coding_interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA61E5E-F024-49A0-B39E-BCDF1CEFF7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD2222AD-B5C9-475A-A4BD-ACD90B9CF5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="354">
   <si>
     <t>Video Solution</t>
   </si>
@@ -1053,6 +1053,40 @@
   <si>
     <t>start from rows and cols that are directly connected to the oceans, set_atl, set_pac and do a dfs from this positions, then return a position if is in both set_a and set_p 
 dfs each cell, keep track of visited, and track which reach pac, atl; dfs on cells adjacent to pac, atl, find overlap of cells that are visited by both pac and atl cells;</t>
+  </si>
+  <si>
+    <t>create a matrix of visited nodes, find 1's in dfs approach after finding all ones in current pass append this to the final list and iterate over rest of coordinates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">create a set of the nums, check if num - 1 in set, if so continue because is not the start of a secuence, if it is not then keep checking if the next value is in the set and increase len, at the end return the max of the lens </t>
+  </si>
+  <si>
+    <t xml:space="preserve">since undirected graph create adj matrix for both nodes, then do a dfs and if neigh == prev node just continue, then check for loops in visited_set and retun if dfs is true and n == len(visited) meaning you traverse the entire graph </t>
+  </si>
+  <si>
+    <t xml:space="preserve">initialzie new head and set tail to this new head, then insert each node from one list into the other comparing the nodes values, in the end check if you still have values in one list and add them and return the new_head.next </t>
+  </si>
+  <si>
+    <t>create a letters_dict and then create a tmp_count dict to get the numbers of chars in each word, use this tupple(sort(tmp_count.items())) as a tupple key for the list_dict and add the words to this dict, , use count of each char in each word as tuple for key in dict, return letters_dict.values()</t>
+  </si>
+  <si>
+    <t>left, right pointers, update left and right until each points at alphanum, compare left and right, continue while left &lt;= right</t>
+  </si>
+  <si>
+    <t>iterate from s[1] and check if this is a palindrome growing to the left and to the right, consider both cases where the palindrome is even and odd</t>
+  </si>
+  <si>
+    <t>recursive(better): if node is none return 0, call same func on left and right, then return max(left, right) + 1 because you need to go up 
+iterative you create a stack of dicts to have the current depth and the current node info, the do a dfs and adding to the stack node.left, depth + 1 same for right</t>
+  </si>
+  <si>
+    <t>recursive dfs on both nodes same time: check if both nodes are none return true, if one is none or the other is none or values  ares different return false, then call on left and right and return left_valid AND right_valid</t>
+  </si>
+  <si>
+    <t>recursive dfs to invert subtrees; bfs to invert levels, use collections.deque; iterative dfs is easy with stack if doing pre-order (Root, left, right) traversal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">traverse root nodes dfs calling same_tree on current node and recursive call is_sub_tree on left and right, return left or right </t>
   </si>
 </sst>
 </file>
@@ -1590,8 +1624,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="D28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2096,7 +2130,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>93</v>
       </c>
@@ -2126,7 +2160,9 @@
       <c r="D31" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="4"/>
+      <c r="E31" s="4" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
@@ -2141,7 +2177,9 @@
       <c r="D32" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="E32" s="4"/>
+      <c r="E32" s="4" t="s">
+        <v>344</v>
+      </c>
     </row>
     <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
@@ -2156,7 +2194,9 @@
       <c r="D33" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="4" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
@@ -2171,7 +2211,9 @@
       <c r="D34" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="E34" s="4"/>
+      <c r="E34" s="4" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
@@ -2246,7 +2288,9 @@
       <c r="D39" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="E39" s="4"/>
+      <c r="E39" s="4" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
@@ -2276,7 +2320,9 @@
       <c r="D41" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="E41" s="4"/>
+      <c r="E41" s="4" t="s">
+        <v>280</v>
+      </c>
     </row>
     <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
@@ -2306,7 +2352,9 @@
       <c r="D43" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="E43" s="4"/>
+      <c r="E43" s="4" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
@@ -2471,7 +2519,9 @@
       <c r="D54" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="E54" s="4"/>
+      <c r="E54" s="4" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="55" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
@@ -2486,7 +2536,9 @@
       <c r="D55" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="E55" s="4"/>
+      <c r="E55" s="4" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="56" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
@@ -2501,7 +2553,9 @@
       <c r="D56" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="E56" s="4"/>
+      <c r="E56" s="4" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="57" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
@@ -2516,7 +2570,9 @@
       <c r="D57" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="E57" s="4"/>
+      <c r="E57" s="4" t="s">
+        <v>348</v>
+      </c>
     </row>
     <row r="58" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
@@ -2531,7 +2587,9 @@
       <c r="D58" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="E58" s="4"/>
+      <c r="E58" s="4" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="59" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
@@ -2561,9 +2619,11 @@
       <c r="D60" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="E60" s="4"/>
-    </row>
-    <row r="61" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="E60" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>190</v>
       </c>
@@ -2576,7 +2636,9 @@
       <c r="D61" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="E61" s="4"/>
+      <c r="E61" s="23" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="62" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
@@ -2588,10 +2650,12 @@
       <c r="C62" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="D62" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="E62" s="4"/>
+      <c r="E62" s="4" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="63" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
@@ -2606,7 +2670,9 @@
       <c r="D63" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="E63" s="4"/>
+      <c r="E63" s="4" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="64" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
@@ -2666,7 +2732,9 @@
       <c r="D67" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="E67" s="4"/>
+      <c r="E67" s="4" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="68" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
@@ -5753,8 +5821,8 @@
   </sheetPr>
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="E43" workbookViewId="0">
+      <selection activeCell="E67" sqref="E67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>